<commit_message>
Refactor authentication handling to improve secrets management and add error handling; update exercises data
</commit_message>
<xml_diff>
--- a/data/exercises.xlsx
+++ b/data/exercises.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workout_Streamlit_Dashboard\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A681838-F9F7-40D3-B935-B2FD8CCB460E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F619726D-300B-4609-8276-112BA7693DAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30612" yWindow="10764" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15264" yWindow="0" windowWidth="15552" windowHeight="16656" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="38">
   <si>
     <t>exercise</t>
   </si>
@@ -64,9 +64,6 @@
     <t>Barbell Row</t>
   </si>
   <si>
-    <t>Back</t>
-  </si>
-  <si>
     <t>Lats</t>
   </si>
   <si>
@@ -113,6 +110,30 @@
   </si>
   <si>
     <t xml:space="preserve">Neutral grip </t>
+  </si>
+  <si>
+    <t>Lateral raise</t>
+  </si>
+  <si>
+    <t>Traps</t>
+  </si>
+  <si>
+    <t>Side delts</t>
+  </si>
+  <si>
+    <t>Helm's row</t>
+  </si>
+  <si>
+    <t>Upper back</t>
+  </si>
+  <si>
+    <t>Hammer curl</t>
+  </si>
+  <si>
+    <t>Bands</t>
+  </si>
+  <si>
+    <t>Single arm pushdown</t>
   </si>
 </sst>
 </file>
@@ -475,16 +496,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -492,7 +514,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -506,7 +528,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -520,7 +542,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
@@ -534,7 +556,7 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
         <v>10</v>
@@ -548,7 +570,7 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
@@ -562,63 +584,63 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" t="s">
         <v>14</v>
-      </c>
-      <c r="D6" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
         <v>16</v>
-      </c>
-      <c r="B7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" t="s">
         <v>19</v>
-      </c>
-      <c r="B9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
@@ -629,16 +651,66 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>30</v>
       </c>
-      <c r="C11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" t="s">
-        <v>17</v>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update exercise data: modified workouts.csv and replaced exercises.xlsx
</commit_message>
<xml_diff>
--- a/data/exercises.xlsx
+++ b/data/exercises.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workout_Streamlit_Dashboard\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F619726D-300B-4609-8276-112BA7693DAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6EE4B1-1141-4C17-863B-D416C7B1D955}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15264" yWindow="0" windowWidth="15552" windowHeight="16656" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="82">
   <si>
     <t>exercise</t>
   </si>
@@ -61,9 +61,6 @@
     <t>Shoulders</t>
   </si>
   <si>
-    <t>Barbell Row</t>
-  </si>
-  <si>
     <t>Lats</t>
   </si>
   <si>
@@ -76,9 +73,6 @@
     <t>Lat Pulldown</t>
   </si>
   <si>
-    <t>Dumbbell Curl</t>
-  </si>
-  <si>
     <t>Forearms</t>
   </si>
   <si>
@@ -106,9 +100,6 @@
     <t>Rope</t>
   </si>
   <si>
-    <t>xx</t>
-  </si>
-  <si>
     <t xml:space="preserve">Neutral grip </t>
   </si>
   <si>
@@ -134,6 +125,147 @@
   </si>
   <si>
     <t>Single arm pushdown</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Goblet Squat</t>
+  </si>
+  <si>
+    <t>Sumo Squat</t>
+  </si>
+  <si>
+    <t>Box</t>
+  </si>
+  <si>
+    <t>Good Morning</t>
+  </si>
+  <si>
+    <t>Close Grip Bench Press</t>
+  </si>
+  <si>
+    <t>Incline Bench Press</t>
+  </si>
+  <si>
+    <t>tertiary_muscle</t>
+  </si>
+  <si>
+    <t>Front delt</t>
+  </si>
+  <si>
+    <t>T-Bar</t>
+  </si>
+  <si>
+    <t>Romanian Deadlift</t>
+  </si>
+  <si>
+    <t>Machine</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Rear delt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Underhand grip </t>
+  </si>
+  <si>
+    <t>Lat pulldown</t>
+  </si>
+  <si>
+    <t>Bicep curl</t>
+  </si>
+  <si>
+    <t>Kettlebell</t>
+  </si>
+  <si>
+    <t>Bar</t>
+  </si>
+  <si>
+    <t>Lateral raise (lying)</t>
+  </si>
+  <si>
+    <t>Shrug</t>
+  </si>
+  <si>
+    <t>Neck</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tibialis raise </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tibialis </t>
+  </si>
+  <si>
+    <t>Wall</t>
+  </si>
+  <si>
+    <t>Leg extension</t>
+  </si>
+  <si>
+    <t>Rear delt raise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rear delts </t>
+  </si>
+  <si>
+    <t>Hip flexor</t>
+  </si>
+  <si>
+    <t>Reverse flye</t>
+  </si>
+  <si>
+    <t>Preacher curl</t>
+  </si>
+  <si>
+    <t>EZ-Bar</t>
+  </si>
+  <si>
+    <t>Incline Curl</t>
+  </si>
+  <si>
+    <t>Triceps push away</t>
+  </si>
+  <si>
+    <t>Neck curl</t>
+  </si>
+  <si>
+    <t>Weighted</t>
+  </si>
+  <si>
+    <t>Manual</t>
+  </si>
+  <si>
+    <t>Neck extension</t>
+  </si>
+  <si>
+    <t>Wrist curl</t>
+  </si>
+  <si>
+    <t>Cable</t>
+  </si>
+  <si>
+    <t>Wrist extension</t>
+  </si>
+  <si>
+    <t>Reverse curl</t>
+  </si>
+  <si>
+    <t>Forearm grippers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metal </t>
+  </si>
+  <si>
+    <t>Leg curl</t>
+  </si>
+  <si>
+    <t>Calf raise</t>
+  </si>
+  <si>
+    <t>Calves</t>
   </si>
 </sst>
 </file>
@@ -496,25 +628,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:E68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="A69" sqref="A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -522,13 +654,16 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -537,180 +672,985 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="E8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
         <v>22</v>
       </c>
-      <c r="C6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" t="s">
-        <v>28</v>
-      </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+      <c r="E9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" t="s">
         <v>20</v>
-      </c>
-      <c r="B10" t="s">
-        <v>27</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
       </c>
       <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="D20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>47</v>
+      </c>
+      <c r="B23" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" t="s">
+        <v>31</v>
+      </c>
+      <c r="D23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E25" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" t="s">
+        <v>15</v>
+      </c>
+      <c r="E27" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" t="s">
+        <v>15</v>
+      </c>
+      <c r="E28" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>50</v>
+      </c>
+      <c r="B29" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" t="s">
+        <v>13</v>
+      </c>
+      <c r="D29" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>50</v>
+      </c>
+      <c r="B30" t="s">
+        <v>49</v>
+      </c>
+      <c r="C30" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30" t="s">
+        <v>15</v>
+      </c>
+      <c r="E30" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>16</v>
+      </c>
+      <c r="B31" t="s">
+        <v>24</v>
+      </c>
+      <c r="C31" t="s">
+        <v>13</v>
+      </c>
+      <c r="D31" t="s">
+        <v>15</v>
+      </c>
+      <c r="E31" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>51</v>
+      </c>
+      <c r="B32" t="s">
+        <v>22</v>
+      </c>
+      <c r="C32" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32" t="s">
         <v>17</v>
       </c>
-      <c r="B11" t="s">
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>51</v>
+      </c>
+      <c r="B33" t="s">
+        <v>20</v>
+      </c>
+      <c r="C33" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>22</v>
+      </c>
+      <c r="C34" t="s">
+        <v>15</v>
+      </c>
+      <c r="D34" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35" t="s">
+        <v>52</v>
+      </c>
+      <c r="C35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D35" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>32</v>
+      </c>
+      <c r="B36" t="s">
+        <v>33</v>
+      </c>
+      <c r="C36" t="s">
+        <v>15</v>
+      </c>
+      <c r="D36" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>18</v>
+      </c>
+      <c r="B37" t="s">
+        <v>25</v>
+      </c>
+      <c r="C37" t="s">
+        <v>8</v>
+      </c>
+      <c r="D37" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>18</v>
+      </c>
+      <c r="B38" t="s">
+        <v>53</v>
+      </c>
+      <c r="C38" t="s">
+        <v>8</v>
+      </c>
+      <c r="D38" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>27</v>
+      </c>
+      <c r="B39" t="s">
+        <v>22</v>
+      </c>
+      <c r="C39" t="s">
         <v>29</v>
       </c>
-      <c r="C11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="D39" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>54</v>
+      </c>
+      <c r="B40" t="s">
+        <v>22</v>
+      </c>
+      <c r="C40" t="s">
+        <v>29</v>
+      </c>
+      <c r="D40" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
         <v>30</v>
       </c>
-      <c r="B12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="B41" t="s">
+        <v>22</v>
+      </c>
+      <c r="C41" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="D41" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>55</v>
+      </c>
+      <c r="B42" t="s">
+        <v>22</v>
+      </c>
+      <c r="C42" t="s">
+        <v>28</v>
+      </c>
+      <c r="D42" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>55</v>
+      </c>
+      <c r="B43" t="s">
+        <v>20</v>
+      </c>
+      <c r="C43" t="s">
+        <v>28</v>
+      </c>
+      <c r="D43" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
         <v>34</v>
       </c>
-      <c r="D13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" t="s">
-        <v>36</v>
-      </c>
-      <c r="C14" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="B44" t="s">
+        <v>25</v>
+      </c>
+      <c r="C44" t="s">
         <v>8</v>
+      </c>
+      <c r="D44" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>57</v>
+      </c>
+      <c r="B45" t="s">
+        <v>52</v>
+      </c>
+      <c r="C45" t="s">
+        <v>58</v>
+      </c>
+      <c r="D45" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>57</v>
+      </c>
+      <c r="B46" t="s">
+        <v>59</v>
+      </c>
+      <c r="C46" t="s">
+        <v>58</v>
+      </c>
+      <c r="D46" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>60</v>
+      </c>
+      <c r="B47" t="s">
+        <v>46</v>
+      </c>
+      <c r="C47" t="s">
+        <v>4</v>
+      </c>
+      <c r="D47" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>6</v>
+      </c>
+      <c r="B48" t="s">
+        <v>46</v>
+      </c>
+      <c r="C48" t="s">
+        <v>7</v>
+      </c>
+      <c r="D48" t="s">
+        <v>8</v>
+      </c>
+      <c r="E48" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>61</v>
+      </c>
+      <c r="B49" t="s">
+        <v>22</v>
+      </c>
+      <c r="C49" t="s">
+        <v>62</v>
+      </c>
+      <c r="D49" t="s">
+        <v>35</v>
+      </c>
+      <c r="E49" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>64</v>
+      </c>
+      <c r="B50" t="s">
+        <v>46</v>
+      </c>
+      <c r="C50" t="s">
+        <v>62</v>
+      </c>
+      <c r="D50" t="s">
+        <v>35</v>
+      </c>
+      <c r="E50" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>65</v>
+      </c>
+      <c r="B51" t="s">
+        <v>66</v>
+      </c>
+      <c r="C51" t="s">
+        <v>15</v>
+      </c>
+      <c r="D51" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>65</v>
+      </c>
+      <c r="B52" t="s">
+        <v>22</v>
+      </c>
+      <c r="C52" t="s">
+        <v>15</v>
+      </c>
+      <c r="D52" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>67</v>
+      </c>
+      <c r="B53" t="s">
+        <v>22</v>
+      </c>
+      <c r="C53" t="s">
+        <v>15</v>
+      </c>
+      <c r="D53" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>68</v>
+      </c>
+      <c r="B54" t="s">
+        <v>25</v>
+      </c>
+      <c r="C54" t="s">
+        <v>8</v>
+      </c>
+      <c r="D54" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>69</v>
+      </c>
+      <c r="B55" t="s">
+        <v>70</v>
+      </c>
+      <c r="C55" t="s">
+        <v>56</v>
+      </c>
+      <c r="D55" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>69</v>
+      </c>
+      <c r="B56" t="s">
+        <v>71</v>
+      </c>
+      <c r="C56" t="s">
+        <v>56</v>
+      </c>
+      <c r="D56" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>72</v>
+      </c>
+      <c r="B57" t="s">
+        <v>70</v>
+      </c>
+      <c r="C57" t="s">
+        <v>56</v>
+      </c>
+      <c r="D57" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>72</v>
+      </c>
+      <c r="B58" t="s">
+        <v>71</v>
+      </c>
+      <c r="C58" t="s">
+        <v>56</v>
+      </c>
+      <c r="D58" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>73</v>
+      </c>
+      <c r="B59" t="s">
+        <v>22</v>
+      </c>
+      <c r="C59" t="s">
+        <v>17</v>
+      </c>
+      <c r="D59" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>73</v>
+      </c>
+      <c r="B60" t="s">
+        <v>20</v>
+      </c>
+      <c r="C60" t="s">
+        <v>17</v>
+      </c>
+      <c r="D60" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>73</v>
+      </c>
+      <c r="B61" t="s">
+        <v>74</v>
+      </c>
+      <c r="C61" t="s">
+        <v>17</v>
+      </c>
+      <c r="D61" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>76</v>
+      </c>
+      <c r="B62" t="s">
+        <v>66</v>
+      </c>
+      <c r="C62" t="s">
+        <v>17</v>
+      </c>
+      <c r="D62" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>75</v>
+      </c>
+      <c r="B63" t="s">
+        <v>22</v>
+      </c>
+      <c r="C63" t="s">
+        <v>17</v>
+      </c>
+      <c r="D63" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>75</v>
+      </c>
+      <c r="B64" t="s">
+        <v>20</v>
+      </c>
+      <c r="C64" t="s">
+        <v>17</v>
+      </c>
+      <c r="D64" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>75</v>
+      </c>
+      <c r="B65" t="s">
+        <v>74</v>
+      </c>
+      <c r="C65" t="s">
+        <v>17</v>
+      </c>
+      <c r="D65" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>77</v>
+      </c>
+      <c r="B66" t="s">
+        <v>78</v>
+      </c>
+      <c r="C66" t="s">
+        <v>17</v>
+      </c>
+      <c r="D66" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>79</v>
+      </c>
+      <c r="B67" t="s">
+        <v>46</v>
+      </c>
+      <c r="C67" t="s">
+        <v>10</v>
+      </c>
+      <c r="D67" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>80</v>
+      </c>
+      <c r="B68" t="s">
+        <v>21</v>
+      </c>
+      <c r="C68" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>